<commit_message>
lpi week done and new leagues
</commit_message>
<xml_diff>
--- a/Game of Yards! 2023.xlsx
+++ b/Game of Yards! 2023.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="33">
   <si>
     <t>Stiff Armed and Dangerous</t>
   </si>
@@ -50,34 +50,16 @@
     <t>Team HebAchi</t>
   </si>
   <si>
-    <t>10-4-0</t>
-  </si>
-  <si>
-    <t>9-5-0</t>
-  </si>
-  <si>
-    <t>5-9-0</t>
-  </si>
-  <si>
-    <t>8-6-0</t>
-  </si>
-  <si>
-    <t>4-10-0</t>
-  </si>
-  <si>
-    <t>7-7-0</t>
-  </si>
-  <si>
-    <t>3-11-0</t>
-  </si>
-  <si>
-    <t>6-8-0</t>
-  </si>
-  <si>
-    <t>2-12-0</t>
-  </si>
-  <si>
-    <t>11-3-0</t>
+    <t>1-2-0</t>
+  </si>
+  <si>
+    <t>0-3-0</t>
+  </si>
+  <si>
+    <t>2-1-0</t>
+  </si>
+  <si>
+    <t>3-0-0</t>
   </si>
   <si>
     <t>Teams</t>
@@ -538,31 +520,31 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -573,31 +555,31 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
       <c r="J3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -608,31 +590,31 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -640,34 +622,34 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="K5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -675,34 +657,34 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -710,34 +692,34 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -745,34 +727,34 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J8" t="s">
         <v>10</v>
       </c>
       <c r="K8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -780,34 +762,34 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" t="s">
-        <v>12</v>
-      </c>
       <c r="K9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -815,34 +797,34 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I10" t="s">
         <v>11</v>
       </c>
       <c r="J10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -850,34 +832,34 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="J11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="K11" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -895,13 +877,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -909,13 +891,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C2">
-        <v>5.4</v>
+        <v>0.8</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -923,13 +905,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>6.4</v>
+        <v>0.9</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -937,13 +919,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>6.7</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -951,10 +933,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>6.8</v>
+        <v>1.3</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -965,13 +947,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>6.8</v>
+        <v>1.4</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -979,13 +961,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>6.9</v>
+        <v>1.6</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -993,13 +975,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>7.4</v>
+        <v>1.8</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1007,13 +989,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>7.8</v>
+        <v>1.9</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1021,13 +1003,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>7.9</v>
+        <v>2.1</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1035,13 +1017,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>7.9</v>
+        <v>2.2</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1059,16 +1041,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1076,16 +1058,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>8.800000000000001</v>
+        <v>2.4</v>
       </c>
       <c r="D2">
-        <v>-1.199999999999999</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1093,16 +1075,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>8.300000000000001</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>-0.6999999999999993</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1110,16 +1092,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>8.300000000000001</v>
+        <v>1.9</v>
       </c>
       <c r="D4">
-        <v>0.3000000000000007</v>
+        <v>-0.1000000000000001</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1127,16 +1109,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>7.6</v>
+        <v>1.6</v>
       </c>
       <c r="D5">
-        <v>-0.4000000000000004</v>
+        <v>-0.3999999999999999</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1144,16 +1126,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>7.4</v>
+        <v>1.6</v>
       </c>
       <c r="D6">
-        <v>-0.5999999999999996</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1161,16 +1143,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>6.6</v>
+        <v>1.3</v>
       </c>
       <c r="D7">
-        <v>0.5999999999999996</v>
+        <v>-0.7</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1178,13 +1160,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>6.5</v>
+        <v>1.2</v>
       </c>
       <c r="D8">
-        <v>1.5</v>
+        <v>-0.8</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -1198,13 +1180,13 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <v>6.2</v>
+        <v>1.1</v>
       </c>
       <c r="D9">
-        <v>1.2</v>
+        <v>0.1000000000000001</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1212,16 +1194,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>5.6</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>-0.4000000000000004</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1229,16 +1211,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>4.7</v>
+        <v>0.9</v>
       </c>
       <c r="D11">
-        <v>-0.2999999999999998</v>
+        <v>-0.09999999999999998</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1256,268 +1238,268 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>30.43</v>
+        <v>38.94</v>
       </c>
       <c r="C2">
-        <v>22.34</v>
+        <v>29.98</v>
       </c>
       <c r="D2">
-        <v>16.75</v>
+        <v>17.23</v>
       </c>
       <c r="E2">
-        <v>11.76</v>
+        <v>8.359999999999999</v>
       </c>
       <c r="F2">
-        <v>8.43</v>
+        <v>3.39</v>
       </c>
       <c r="G2">
-        <v>5.390000000000001</v>
+        <v>1.27</v>
       </c>
       <c r="H2">
-        <v>2.97</v>
+        <v>0.5700000000000001</v>
       </c>
       <c r="I2">
-        <v>1.42</v>
+        <v>0.21</v>
       </c>
       <c r="J2">
-        <v>0.46</v>
+        <v>0.05</v>
       </c>
       <c r="K2">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>95.10000000000001</v>
+        <v>99.17</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>24.11</v>
+        <v>34.06</v>
       </c>
       <c r="C3">
-        <v>20.43</v>
+        <v>26.93</v>
       </c>
       <c r="D3">
-        <v>16.82</v>
+        <v>18.71</v>
       </c>
       <c r="E3">
-        <v>14.06</v>
+        <v>10.71</v>
       </c>
       <c r="F3">
-        <v>9.890000000000001</v>
+        <v>5.4</v>
       </c>
       <c r="G3">
-        <v>7.489999999999999</v>
+        <v>2.41</v>
       </c>
       <c r="H3">
-        <v>4.3</v>
+        <v>1.1</v>
       </c>
       <c r="I3">
-        <v>1.92</v>
+        <v>0.5700000000000001</v>
       </c>
       <c r="J3">
-        <v>0.8699999999999999</v>
+        <v>0.11</v>
       </c>
       <c r="K3">
-        <v>0.11</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>92.8</v>
+        <v>98.22</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>20.58</v>
+        <v>17.99</v>
       </c>
       <c r="C4">
-        <v>21.85</v>
+        <v>21</v>
       </c>
       <c r="D4">
-        <v>19.43</v>
+        <v>21.23</v>
       </c>
       <c r="E4">
-        <v>15.17</v>
+        <v>16.22</v>
       </c>
       <c r="F4">
-        <v>10.04</v>
+        <v>10.22</v>
       </c>
       <c r="G4">
-        <v>6.69</v>
+        <v>6.600000000000001</v>
       </c>
       <c r="H4">
-        <v>3.89</v>
+        <v>3.77</v>
       </c>
       <c r="I4">
-        <v>1.72</v>
+        <v>2.13</v>
       </c>
       <c r="J4">
-        <v>0.5700000000000001</v>
+        <v>0.7799999999999999</v>
       </c>
       <c r="K4">
         <v>0.06</v>
       </c>
       <c r="L4">
-        <v>93.76000000000001</v>
+        <v>93.25999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>10.03</v>
+        <v>4.23</v>
       </c>
       <c r="C5">
-        <v>11.74</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="D5">
-        <v>13.9</v>
+        <v>14.18</v>
       </c>
       <c r="E5">
-        <v>14.23</v>
+        <v>15.97</v>
       </c>
       <c r="F5">
-        <v>15.48</v>
+        <v>15.55</v>
       </c>
       <c r="G5">
-        <v>13.66</v>
+        <v>14.28</v>
       </c>
       <c r="H5">
-        <v>10.22</v>
+        <v>11.83</v>
       </c>
       <c r="I5">
-        <v>6.75</v>
+        <v>9.120000000000001</v>
       </c>
       <c r="J5">
-        <v>3.28</v>
+        <v>5.7</v>
       </c>
       <c r="K5">
-        <v>0.7100000000000001</v>
+        <v>0.84</v>
       </c>
       <c r="L5">
-        <v>79.04000000000001</v>
+        <v>72.51000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>7.94</v>
+        <v>1.97</v>
       </c>
       <c r="C6">
-        <v>10.9</v>
+        <v>5.2</v>
       </c>
       <c r="D6">
-        <v>12.72</v>
+        <v>8.99</v>
       </c>
       <c r="E6">
-        <v>14.33</v>
+        <v>13.01</v>
       </c>
       <c r="F6">
-        <v>15.1</v>
+        <v>15.15</v>
       </c>
       <c r="G6">
-        <v>14.08</v>
+        <v>15.86</v>
       </c>
       <c r="H6">
-        <v>11.13</v>
+        <v>14.59</v>
       </c>
       <c r="I6">
-        <v>8.129999999999999</v>
+        <v>13.07</v>
       </c>
       <c r="J6">
-        <v>4.53</v>
+        <v>10.36</v>
       </c>
       <c r="K6">
-        <v>1.14</v>
+        <v>1.8</v>
       </c>
       <c r="L6">
-        <v>75.07000000000001</v>
+        <v>60.18</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>4.95</v>
+        <v>1.6</v>
       </c>
       <c r="C7">
-        <v>7.82</v>
+        <v>4.24</v>
       </c>
       <c r="D7">
-        <v>10.57</v>
+        <v>8.720000000000001</v>
       </c>
       <c r="E7">
-        <v>13.52</v>
+        <v>12.72</v>
       </c>
       <c r="F7">
-        <v>14.84</v>
+        <v>14.97</v>
       </c>
       <c r="G7">
-        <v>14.46</v>
+        <v>15.51</v>
       </c>
       <c r="H7">
-        <v>13.95</v>
+        <v>15.3</v>
       </c>
       <c r="I7">
-        <v>10.76</v>
+        <v>13.45</v>
       </c>
       <c r="J7">
-        <v>7.149999999999999</v>
+        <v>10.99</v>
       </c>
       <c r="K7">
-        <v>1.98</v>
+        <v>2.5</v>
       </c>
       <c r="L7">
-        <v>66.16</v>
+        <v>57.76</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1525,151 +1507,151 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>1.31</v>
+        <v>0.58</v>
       </c>
       <c r="C8">
-        <v>2.97</v>
+        <v>2.23</v>
       </c>
       <c r="D8">
-        <v>5.149999999999999</v>
+        <v>4.91</v>
       </c>
       <c r="E8">
-        <v>8.450000000000001</v>
+        <v>9.81</v>
       </c>
       <c r="F8">
-        <v>11.64</v>
+        <v>14.13</v>
       </c>
       <c r="G8">
-        <v>14.39</v>
+        <v>15.47</v>
       </c>
       <c r="H8">
-        <v>17.03</v>
+        <v>17.25</v>
       </c>
       <c r="I8">
-        <v>17.92</v>
+        <v>16.91</v>
       </c>
       <c r="J8">
-        <v>14.98</v>
+        <v>14.28</v>
       </c>
       <c r="K8">
-        <v>6.16</v>
+        <v>4.43</v>
       </c>
       <c r="L8">
-        <v>43.91</v>
+        <v>47.13</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>0.53</v>
+        <v>0.33</v>
       </c>
       <c r="C9">
-        <v>1.3</v>
+        <v>1.27</v>
       </c>
       <c r="D9">
-        <v>2.92</v>
+        <v>3.25</v>
       </c>
       <c r="E9">
-        <v>4.84</v>
+        <v>6.41</v>
       </c>
       <c r="F9">
-        <v>7.91</v>
+        <v>10.31</v>
       </c>
       <c r="G9">
-        <v>11.89</v>
+        <v>13.31</v>
       </c>
       <c r="H9">
-        <v>16.64</v>
+        <v>16.28</v>
       </c>
       <c r="I9">
-        <v>20.68</v>
+        <v>19.49</v>
       </c>
       <c r="J9">
-        <v>21.73</v>
+        <v>21.97</v>
       </c>
       <c r="K9">
-        <v>11.56</v>
+        <v>7.380000000000001</v>
       </c>
       <c r="L9">
-        <v>29.39</v>
+        <v>34.88</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B10">
-        <v>0.12</v>
+        <v>0.3</v>
       </c>
       <c r="C10">
-        <v>0.62</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="D10">
-        <v>1.67</v>
+        <v>2.77</v>
       </c>
       <c r="E10">
-        <v>3.51</v>
+        <v>6.74</v>
       </c>
       <c r="F10">
-        <v>6.140000000000001</v>
+        <v>10.62</v>
       </c>
       <c r="G10">
-        <v>10.54</v>
+        <v>14.58</v>
       </c>
       <c r="H10">
-        <v>16.14</v>
+        <v>17.44</v>
       </c>
       <c r="I10">
-        <v>21.24</v>
+        <v>19.81</v>
       </c>
       <c r="J10">
-        <v>24.47</v>
+        <v>19.66</v>
       </c>
       <c r="K10">
-        <v>15.55</v>
+        <v>7.23</v>
       </c>
       <c r="L10">
-        <v>22.6</v>
+        <v>35.86</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0.06999999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="E11">
-        <v>0.13</v>
+        <v>0.05</v>
       </c>
       <c r="F11">
-        <v>0.53</v>
+        <v>0.26</v>
       </c>
       <c r="G11">
-        <v>1.41</v>
+        <v>0.7100000000000001</v>
       </c>
       <c r="H11">
-        <v>3.73</v>
+        <v>1.87</v>
       </c>
       <c r="I11">
-        <v>9.460000000000001</v>
+        <v>5.24</v>
       </c>
       <c r="J11">
-        <v>21.96</v>
+        <v>16.1</v>
       </c>
       <c r="K11">
-        <v>62.68</v>
+        <v>75.76000000000001</v>
       </c>
       <c r="L11">
-        <v>2.17</v>
+        <v>1.03</v>
       </c>
     </row>
   </sheetData>
@@ -1687,16 +1669,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1704,13 +1686,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1721,13 +1703,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1738,13 +1720,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1755,10 +1737,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -1772,13 +1754,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1789,13 +1771,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C7">
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1806,7 +1788,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>-7</v>
@@ -1823,13 +1805,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>-10</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1840,13 +1822,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>-14</v>
+        <v>-10</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1857,13 +1839,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>-37</v>
+        <v>-16</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E11">
         <v>0</v>

</xml_diff>